<commit_message>
Almost Finished part 1 of assignment
</commit_message>
<xml_diff>
--- a/data/DataInExcel.xlsx
+++ b/data/DataInExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mvb00\PycharmProjects\SAALAB\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magnus\Documents\GitHub\saa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D2E847-D90A-40F0-A8DD-AC674FA369CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C38419-0258-4413-B4A6-63A2B59FC5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{65057805-D743-4487-9EE5-C0194F39D916}"/>
+    <workbookView xWindow="9165" yWindow="8340" windowWidth="28800" windowHeight="15345" xr2:uid="{65057805-D743-4487-9EE5-C0194F39D916}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>InputVoltage</t>
   </si>
   <si>
-    <t>Displacment(deg)</t>
-  </si>
-  <si>
     <t>Voltage(mv)</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>backward</t>
+  </si>
+  <si>
+    <t>Displacement(deg)</t>
   </si>
 </sst>
 </file>
@@ -421,21 +421,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEA5147-2EB8-4927-B2B4-D9F71C85541E}">
   <dimension ref="A1:I249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="B220" sqref="B220:B249"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" customHeight="1">
+    <row r="1" spans="1:9" ht="14.1" customHeight="1">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -443,10 +443,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="1"/>
@@ -456,7 +456,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -472,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>10</v>
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>20</v>
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2">
         <v>30</v>
@@ -514,7 +514,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2">
         <v>40</v>
@@ -528,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2">
         <v>50</v>
@@ -542,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2">
         <v>60</v>
@@ -556,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2">
         <v>70</v>
@@ -570,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2">
         <v>80</v>
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2">
         <v>90</v>
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2">
         <v>100</v>
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2">
         <v>110</v>
@@ -626,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2">
         <v>120</v>
@@ -640,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2">
         <v>130</v>
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2">
         <v>140</v>
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2">
         <v>150</v>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2">
         <v>160</v>
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2">
         <v>170</v>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="2">
         <v>180</v>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2">
         <v>190</v>
@@ -738,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="2">
         <v>200</v>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" s="2">
         <v>210</v>
@@ -766,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2">
         <v>220</v>
@@ -780,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" s="2">
         <v>230</v>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" s="2">
         <v>240</v>
@@ -808,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2">
         <v>250</v>
@@ -822,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="2">
         <v>260</v>
@@ -836,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" s="2">
         <v>270</v>
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="2">
         <v>280</v>
@@ -864,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31" s="2">
         <v>290</v>
@@ -878,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" s="2">
         <v>300</v>
@@ -892,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
@@ -906,7 +906,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34" s="2">
         <v>10</v>
@@ -920,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" s="2">
         <v>20</v>
@@ -934,7 +934,7 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" s="2">
         <v>30</v>
@@ -948,7 +948,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37" s="2">
         <v>40</v>
@@ -962,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38" s="2">
         <v>50</v>
@@ -976,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" s="2">
         <v>60</v>
@@ -990,7 +990,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40" s="2">
         <v>70</v>
@@ -1004,7 +1004,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" s="2">
         <v>80</v>
@@ -1018,7 +1018,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2">
         <v>90</v>
@@ -1032,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43" s="2">
         <v>100</v>
@@ -1046,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" s="2">
         <v>110</v>
@@ -1060,7 +1060,7 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45" s="2">
         <v>120</v>
@@ -1074,7 +1074,7 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" s="2">
         <v>130</v>
@@ -1088,7 +1088,7 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47" s="2">
         <v>140</v>
@@ -1102,7 +1102,7 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" s="2">
         <v>150</v>
@@ -1116,7 +1116,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" s="2">
         <v>160</v>
@@ -1130,7 +1130,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50" s="2">
         <v>170</v>
@@ -1144,7 +1144,7 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" s="2">
         <v>180</v>
@@ -1158,7 +1158,7 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" s="2">
         <v>190</v>
@@ -1172,7 +1172,7 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53" s="2">
         <v>200</v>
@@ -1186,7 +1186,7 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C54" s="2">
         <v>210</v>
@@ -1200,7 +1200,7 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C55" s="2">
         <v>220</v>
@@ -1214,7 +1214,7 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56" s="2">
         <v>230</v>
@@ -1228,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C57" s="2">
         <v>240</v>
@@ -1242,7 +1242,7 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58" s="2">
         <v>250</v>
@@ -1256,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C59" s="2">
         <v>260</v>
@@ -1270,7 +1270,7 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60" s="2">
         <v>270</v>
@@ -1284,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61" s="2">
         <v>280</v>
@@ -1298,7 +1298,7 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C62" s="2">
         <v>290</v>
@@ -1312,7 +1312,7 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63" s="2">
         <v>300</v>
@@ -1326,7 +1326,7 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64" s="2">
         <v>0</v>
@@ -1340,7 +1340,7 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C65" s="2">
         <v>10</v>
@@ -1354,7 +1354,7 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C66" s="2">
         <v>20</v>
@@ -1368,7 +1368,7 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C67" s="2">
         <v>30</v>
@@ -1382,7 +1382,7 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C68" s="2">
         <v>40</v>
@@ -1396,7 +1396,7 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" s="2">
         <v>50</v>
@@ -1410,7 +1410,7 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70" s="2">
         <v>60</v>
@@ -1424,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71" s="2">
         <v>70</v>
@@ -1438,7 +1438,7 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72" s="2">
         <v>80</v>
@@ -1452,7 +1452,7 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73" s="2">
         <v>90</v>
@@ -1466,7 +1466,7 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C74" s="2">
         <v>100</v>
@@ -1480,7 +1480,7 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C75" s="2">
         <v>110</v>
@@ -1494,7 +1494,7 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C76" s="2">
         <v>120</v>
@@ -1508,7 +1508,7 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C77" s="2">
         <v>130</v>
@@ -1522,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C78" s="2">
         <v>140</v>
@@ -1536,7 +1536,7 @@
         <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C79" s="2">
         <v>150</v>
@@ -1550,7 +1550,7 @@
         <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C80" s="2">
         <v>160</v>
@@ -1564,7 +1564,7 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C81" s="2">
         <v>170</v>
@@ -1578,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C82" s="2">
         <v>180</v>
@@ -1592,7 +1592,7 @@
         <v>10</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C83" s="2">
         <v>190</v>
@@ -1606,7 +1606,7 @@
         <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C84" s="2">
         <v>200</v>
@@ -1620,7 +1620,7 @@
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C85" s="2">
         <v>210</v>
@@ -1634,7 +1634,7 @@
         <v>10</v>
       </c>
       <c r="B86" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C86" s="2">
         <v>220</v>
@@ -1648,7 +1648,7 @@
         <v>10</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C87" s="2">
         <v>230</v>
@@ -1662,7 +1662,7 @@
         <v>10</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C88" s="2">
         <v>240</v>
@@ -1676,7 +1676,7 @@
         <v>10</v>
       </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C89" s="2">
         <v>250</v>
@@ -1690,7 +1690,7 @@
         <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C90" s="2">
         <v>260</v>
@@ -1704,7 +1704,7 @@
         <v>10</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C91" s="2">
         <v>270</v>
@@ -1718,7 +1718,7 @@
         <v>10</v>
       </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C92" s="2">
         <v>280</v>
@@ -1732,7 +1732,7 @@
         <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C93" s="2">
         <v>290</v>
@@ -1746,7 +1746,7 @@
         <v>10</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C94" s="2">
         <v>300</v>
@@ -1760,7 +1760,7 @@
         <v>10</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C95" s="2">
         <v>300</v>
@@ -1774,7 +1774,7 @@
         <v>10</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C96" s="2">
         <v>290</v>
@@ -1788,7 +1788,7 @@
         <v>10</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C97" s="2">
         <v>280</v>
@@ -1802,7 +1802,7 @@
         <v>10</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C98" s="2">
         <v>270</v>
@@ -1816,7 +1816,7 @@
         <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C99" s="2">
         <v>260</v>
@@ -1830,7 +1830,7 @@
         <v>10</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C100" s="2">
         <v>250</v>
@@ -1844,7 +1844,7 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C101" s="2">
         <v>240</v>
@@ -1858,7 +1858,7 @@
         <v>10</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C102" s="2">
         <v>230</v>
@@ -1872,7 +1872,7 @@
         <v>10</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C103" s="2">
         <v>220</v>
@@ -1886,7 +1886,7 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C104" s="2">
         <v>210</v>
@@ -1900,7 +1900,7 @@
         <v>10</v>
       </c>
       <c r="B105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C105" s="2">
         <v>200</v>
@@ -1914,7 +1914,7 @@
         <v>10</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C106" s="2">
         <v>190</v>
@@ -1928,7 +1928,7 @@
         <v>10</v>
       </c>
       <c r="B107" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C107" s="2">
         <v>180</v>
@@ -1942,7 +1942,7 @@
         <v>10</v>
       </c>
       <c r="B108" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C108" s="2">
         <v>170</v>
@@ -1956,7 +1956,7 @@
         <v>10</v>
       </c>
       <c r="B109" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C109" s="2">
         <v>160</v>
@@ -1970,7 +1970,7 @@
         <v>10</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C110" s="2">
         <v>150</v>
@@ -1984,7 +1984,7 @@
         <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C111" s="2">
         <v>140</v>
@@ -1998,7 +1998,7 @@
         <v>10</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C112" s="2">
         <v>130</v>
@@ -2012,7 +2012,7 @@
         <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C113" s="2">
         <v>120</v>
@@ -2026,7 +2026,7 @@
         <v>10</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C114" s="2">
         <v>110</v>
@@ -2040,7 +2040,7 @@
         <v>10</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C115" s="2">
         <v>100</v>
@@ -2054,7 +2054,7 @@
         <v>10</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C116" s="2">
         <v>90</v>
@@ -2068,7 +2068,7 @@
         <v>10</v>
       </c>
       <c r="B117" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C117" s="2">
         <v>80</v>
@@ -2082,7 +2082,7 @@
         <v>10</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C118" s="2">
         <v>70</v>
@@ -2096,7 +2096,7 @@
         <v>10</v>
       </c>
       <c r="B119" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C119" s="2">
         <v>60</v>
@@ -2110,7 +2110,7 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C120" s="2">
         <v>50</v>
@@ -2124,7 +2124,7 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C121" s="2">
         <v>40</v>
@@ -2138,7 +2138,7 @@
         <v>10</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C122" s="2">
         <v>30</v>
@@ -2152,7 +2152,7 @@
         <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C123" s="2">
         <v>20</v>
@@ -2166,7 +2166,7 @@
         <v>10</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C124" s="2">
         <v>10</v>
@@ -2180,7 +2180,7 @@
         <v>10</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C125" s="2">
         <v>0</v>
@@ -2194,7 +2194,7 @@
         <v>10</v>
       </c>
       <c r="B126" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C126" s="2">
         <v>0</v>
@@ -2208,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="B127" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C127" s="2">
         <v>10</v>
@@ -2222,7 +2222,7 @@
         <v>10</v>
       </c>
       <c r="B128" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C128" s="2">
         <v>20</v>
@@ -2236,7 +2236,7 @@
         <v>10</v>
       </c>
       <c r="B129" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C129" s="2">
         <v>30</v>
@@ -2250,7 +2250,7 @@
         <v>10</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C130" s="2">
         <v>40</v>
@@ -2264,7 +2264,7 @@
         <v>10</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C131" s="2">
         <v>50</v>
@@ -2278,7 +2278,7 @@
         <v>10</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C132" s="2">
         <v>60</v>
@@ -2292,7 +2292,7 @@
         <v>10</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C133" s="2">
         <v>70</v>
@@ -2306,7 +2306,7 @@
         <v>10</v>
       </c>
       <c r="B134" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C134" s="2">
         <v>80</v>
@@ -2320,7 +2320,7 @@
         <v>10</v>
       </c>
       <c r="B135" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C135" s="2">
         <v>90</v>
@@ -2334,7 +2334,7 @@
         <v>10</v>
       </c>
       <c r="B136" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C136" s="2">
         <v>100</v>
@@ -2348,7 +2348,7 @@
         <v>10</v>
       </c>
       <c r="B137" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C137" s="2">
         <v>110</v>
@@ -2362,7 +2362,7 @@
         <v>10</v>
       </c>
       <c r="B138" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C138" s="2">
         <v>120</v>
@@ -2376,7 +2376,7 @@
         <v>10</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C139" s="2">
         <v>130</v>
@@ -2390,7 +2390,7 @@
         <v>10</v>
       </c>
       <c r="B140" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C140" s="2">
         <v>140</v>
@@ -2404,7 +2404,7 @@
         <v>10</v>
       </c>
       <c r="B141" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C141" s="2">
         <v>150</v>
@@ -2418,7 +2418,7 @@
         <v>10</v>
       </c>
       <c r="B142" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C142" s="2">
         <v>160</v>
@@ -2432,7 +2432,7 @@
         <v>10</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C143" s="2">
         <v>170</v>
@@ -2446,7 +2446,7 @@
         <v>10</v>
       </c>
       <c r="B144" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C144" s="2">
         <v>180</v>
@@ -2460,7 +2460,7 @@
         <v>10</v>
       </c>
       <c r="B145" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C145" s="2">
         <v>190</v>
@@ -2474,7 +2474,7 @@
         <v>10</v>
       </c>
       <c r="B146" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C146" s="2">
         <v>200</v>
@@ -2488,7 +2488,7 @@
         <v>10</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C147" s="2">
         <v>210</v>
@@ -2502,7 +2502,7 @@
         <v>10</v>
       </c>
       <c r="B148" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C148" s="2">
         <v>220</v>
@@ -2516,7 +2516,7 @@
         <v>10</v>
       </c>
       <c r="B149" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C149" s="2">
         <v>230</v>
@@ -2530,7 +2530,7 @@
         <v>10</v>
       </c>
       <c r="B150" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C150" s="2">
         <v>240</v>
@@ -2544,7 +2544,7 @@
         <v>10</v>
       </c>
       <c r="B151" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C151" s="2">
         <v>250</v>
@@ -2558,7 +2558,7 @@
         <v>10</v>
       </c>
       <c r="B152" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C152" s="2">
         <v>260</v>
@@ -2572,7 +2572,7 @@
         <v>10</v>
       </c>
       <c r="B153" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C153" s="2">
         <v>270</v>
@@ -2586,7 +2586,7 @@
         <v>10</v>
       </c>
       <c r="B154" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C154" s="2">
         <v>280</v>
@@ -2600,7 +2600,7 @@
         <v>10</v>
       </c>
       <c r="B155" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C155" s="2">
         <v>290</v>
@@ -2614,7 +2614,7 @@
         <v>10</v>
       </c>
       <c r="B156" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C156" s="2">
         <v>300</v>
@@ -2628,7 +2628,7 @@
         <v>10</v>
       </c>
       <c r="B157" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C157" s="2">
         <v>300</v>
@@ -2642,7 +2642,7 @@
         <v>10</v>
       </c>
       <c r="B158" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C158" s="2">
         <v>290</v>
@@ -2656,7 +2656,7 @@
         <v>10</v>
       </c>
       <c r="B159" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C159" s="2">
         <v>280</v>
@@ -2670,7 +2670,7 @@
         <v>10</v>
       </c>
       <c r="B160" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C160" s="2">
         <v>270</v>
@@ -2684,7 +2684,7 @@
         <v>10</v>
       </c>
       <c r="B161" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C161" s="2">
         <v>260</v>
@@ -2698,7 +2698,7 @@
         <v>10</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C162" s="2">
         <v>250</v>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="B163" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C163" s="2">
         <v>240</v>
@@ -2726,7 +2726,7 @@
         <v>10</v>
       </c>
       <c r="B164" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C164" s="2">
         <v>230</v>
@@ -2740,7 +2740,7 @@
         <v>10</v>
       </c>
       <c r="B165" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C165" s="2">
         <v>220</v>
@@ -2754,7 +2754,7 @@
         <v>10</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C166" s="2">
         <v>210</v>
@@ -2768,7 +2768,7 @@
         <v>10</v>
       </c>
       <c r="B167" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C167" s="2">
         <v>200</v>
@@ -2782,7 +2782,7 @@
         <v>10</v>
       </c>
       <c r="B168" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C168" s="2">
         <v>190</v>
@@ -2796,7 +2796,7 @@
         <v>10</v>
       </c>
       <c r="B169" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C169" s="2">
         <v>180</v>
@@ -2810,7 +2810,7 @@
         <v>10</v>
       </c>
       <c r="B170" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C170" s="2">
         <v>170</v>
@@ -2824,7 +2824,7 @@
         <v>10</v>
       </c>
       <c r="B171" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C171" s="2">
         <v>160</v>
@@ -2838,7 +2838,7 @@
         <v>10</v>
       </c>
       <c r="B172" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C172" s="2">
         <v>150</v>
@@ -2852,7 +2852,7 @@
         <v>10</v>
       </c>
       <c r="B173" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C173" s="2">
         <v>140</v>
@@ -2866,7 +2866,7 @@
         <v>10</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C174" s="2">
         <v>130</v>
@@ -2880,7 +2880,7 @@
         <v>10</v>
       </c>
       <c r="B175" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C175" s="2">
         <v>120</v>
@@ -2894,7 +2894,7 @@
         <v>10</v>
       </c>
       <c r="B176" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C176" s="2">
         <v>110</v>
@@ -2908,7 +2908,7 @@
         <v>10</v>
       </c>
       <c r="B177" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C177" s="2">
         <v>100</v>
@@ -2922,7 +2922,7 @@
         <v>10</v>
       </c>
       <c r="B178" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C178" s="2">
         <v>90</v>
@@ -2936,7 +2936,7 @@
         <v>10</v>
       </c>
       <c r="B179" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C179" s="2">
         <v>80</v>
@@ -2950,7 +2950,7 @@
         <v>10</v>
       </c>
       <c r="B180" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C180" s="2">
         <v>70</v>
@@ -2964,7 +2964,7 @@
         <v>10</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C181" s="2">
         <v>60</v>
@@ -2978,7 +2978,7 @@
         <v>10</v>
       </c>
       <c r="B182" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C182" s="2">
         <v>50</v>
@@ -2992,7 +2992,7 @@
         <v>10</v>
       </c>
       <c r="B183" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C183" s="2">
         <v>40</v>
@@ -3006,7 +3006,7 @@
         <v>10</v>
       </c>
       <c r="B184" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C184" s="2">
         <v>30</v>
@@ -3020,7 +3020,7 @@
         <v>10</v>
       </c>
       <c r="B185" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C185" s="2">
         <v>20</v>
@@ -3034,7 +3034,7 @@
         <v>10</v>
       </c>
       <c r="B186" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C186" s="2">
         <v>10</v>
@@ -3048,7 +3048,7 @@
         <v>10</v>
       </c>
       <c r="B187" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C187" s="2">
         <v>0</v>
@@ -3062,7 +3062,7 @@
         <v>10</v>
       </c>
       <c r="B188" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C188" s="2">
         <v>0</v>
@@ -3076,7 +3076,7 @@
         <v>10</v>
       </c>
       <c r="B189" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C189" s="2">
         <v>10</v>
@@ -3090,7 +3090,7 @@
         <v>10</v>
       </c>
       <c r="B190" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C190" s="2">
         <v>20</v>
@@ -3104,7 +3104,7 @@
         <v>10</v>
       </c>
       <c r="B191" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C191" s="2">
         <v>30</v>
@@ -3118,7 +3118,7 @@
         <v>10</v>
       </c>
       <c r="B192" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C192" s="2">
         <v>40</v>
@@ -3132,7 +3132,7 @@
         <v>10</v>
       </c>
       <c r="B193" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C193" s="2">
         <v>50</v>
@@ -3146,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="B194" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C194" s="2">
         <v>60</v>
@@ -3160,7 +3160,7 @@
         <v>10</v>
       </c>
       <c r="B195" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C195" s="2">
         <v>70</v>
@@ -3174,7 +3174,7 @@
         <v>10</v>
       </c>
       <c r="B196" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C196" s="2">
         <v>80</v>
@@ -3188,7 +3188,7 @@
         <v>10</v>
       </c>
       <c r="B197" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C197" s="2">
         <v>90</v>
@@ -3202,7 +3202,7 @@
         <v>10</v>
       </c>
       <c r="B198" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C198" s="2">
         <v>100</v>
@@ -3216,7 +3216,7 @@
         <v>10</v>
       </c>
       <c r="B199" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C199" s="2">
         <v>110</v>
@@ -3230,7 +3230,7 @@
         <v>10</v>
       </c>
       <c r="B200" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C200" s="2">
         <v>120</v>
@@ -3244,7 +3244,7 @@
         <v>10</v>
       </c>
       <c r="B201" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C201" s="2">
         <v>130</v>
@@ -3258,7 +3258,7 @@
         <v>10</v>
       </c>
       <c r="B202" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C202" s="2">
         <v>140</v>
@@ -3272,7 +3272,7 @@
         <v>10</v>
       </c>
       <c r="B203" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C203" s="2">
         <v>150</v>
@@ -3286,7 +3286,7 @@
         <v>10</v>
       </c>
       <c r="B204" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C204" s="2">
         <v>160</v>
@@ -3300,7 +3300,7 @@
         <v>10</v>
       </c>
       <c r="B205" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C205" s="2">
         <v>170</v>
@@ -3314,7 +3314,7 @@
         <v>10</v>
       </c>
       <c r="B206" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C206" s="2">
         <v>180</v>
@@ -3328,7 +3328,7 @@
         <v>10</v>
       </c>
       <c r="B207" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C207" s="2">
         <v>190</v>
@@ -3342,7 +3342,7 @@
         <v>10</v>
       </c>
       <c r="B208" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C208" s="2">
         <v>200</v>
@@ -3356,7 +3356,7 @@
         <v>10</v>
       </c>
       <c r="B209" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C209" s="2">
         <v>210</v>
@@ -3370,7 +3370,7 @@
         <v>10</v>
       </c>
       <c r="B210" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C210" s="2">
         <v>220</v>
@@ -3384,7 +3384,7 @@
         <v>10</v>
       </c>
       <c r="B211" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C211" s="2">
         <v>230</v>
@@ -3398,7 +3398,7 @@
         <v>10</v>
       </c>
       <c r="B212" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C212" s="2">
         <v>240</v>
@@ -3412,7 +3412,7 @@
         <v>10</v>
       </c>
       <c r="B213" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C213" s="2">
         <v>250</v>
@@ -3426,7 +3426,7 @@
         <v>10</v>
       </c>
       <c r="B214" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C214" s="2">
         <v>260</v>
@@ -3440,7 +3440,7 @@
         <v>10</v>
       </c>
       <c r="B215" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C215" s="2">
         <v>270</v>
@@ -3454,7 +3454,7 @@
         <v>10</v>
       </c>
       <c r="B216" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C216" s="2">
         <v>280</v>
@@ -3468,7 +3468,7 @@
         <v>10</v>
       </c>
       <c r="B217" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C217" s="2">
         <v>290</v>
@@ -3482,7 +3482,7 @@
         <v>10</v>
       </c>
       <c r="B218" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C218" s="2">
         <v>300</v>
@@ -3496,7 +3496,7 @@
         <v>10</v>
       </c>
       <c r="B219" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C219" s="2">
         <v>300</v>
@@ -3510,7 +3510,7 @@
         <v>10</v>
       </c>
       <c r="B220" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C220" s="2">
         <v>290</v>
@@ -3524,7 +3524,7 @@
         <v>10</v>
       </c>
       <c r="B221" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C221" s="2">
         <v>280</v>
@@ -3538,7 +3538,7 @@
         <v>10</v>
       </c>
       <c r="B222" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C222" s="2">
         <v>270</v>
@@ -3552,7 +3552,7 @@
         <v>10</v>
       </c>
       <c r="B223" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C223" s="2">
         <v>260</v>
@@ -3566,7 +3566,7 @@
         <v>10</v>
       </c>
       <c r="B224" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C224" s="2">
         <v>250</v>
@@ -3580,7 +3580,7 @@
         <v>10</v>
       </c>
       <c r="B225" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C225" s="2">
         <v>240</v>
@@ -3594,7 +3594,7 @@
         <v>10</v>
       </c>
       <c r="B226" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C226" s="2">
         <v>230</v>
@@ -3608,7 +3608,7 @@
         <v>10</v>
       </c>
       <c r="B227" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C227" s="2">
         <v>220</v>
@@ -3622,7 +3622,7 @@
         <v>10</v>
       </c>
       <c r="B228" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C228" s="2">
         <v>210</v>
@@ -3636,7 +3636,7 @@
         <v>10</v>
       </c>
       <c r="B229" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C229" s="2">
         <v>200</v>
@@ -3650,7 +3650,7 @@
         <v>10</v>
       </c>
       <c r="B230" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C230" s="2">
         <v>190</v>
@@ -3664,7 +3664,7 @@
         <v>10</v>
       </c>
       <c r="B231" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C231" s="2">
         <v>180</v>
@@ -3678,7 +3678,7 @@
         <v>10</v>
       </c>
       <c r="B232" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C232" s="2">
         <v>170</v>
@@ -3692,7 +3692,7 @@
         <v>10</v>
       </c>
       <c r="B233" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C233" s="2">
         <v>160</v>
@@ -3706,7 +3706,7 @@
         <v>10</v>
       </c>
       <c r="B234" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C234" s="2">
         <v>150</v>
@@ -3720,7 +3720,7 @@
         <v>10</v>
       </c>
       <c r="B235" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C235" s="2">
         <v>140</v>
@@ -3734,7 +3734,7 @@
         <v>10</v>
       </c>
       <c r="B236" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C236" s="2">
         <v>130</v>
@@ -3748,7 +3748,7 @@
         <v>10</v>
       </c>
       <c r="B237" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C237" s="2">
         <v>120</v>
@@ -3762,7 +3762,7 @@
         <v>10</v>
       </c>
       <c r="B238" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C238" s="2">
         <v>110</v>
@@ -3776,7 +3776,7 @@
         <v>10</v>
       </c>
       <c r="B239" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C239" s="2">
         <v>100</v>
@@ -3790,7 +3790,7 @@
         <v>10</v>
       </c>
       <c r="B240" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C240" s="2">
         <v>90</v>
@@ -3804,7 +3804,7 @@
         <v>10</v>
       </c>
       <c r="B241" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C241" s="2">
         <v>80</v>
@@ -3818,7 +3818,7 @@
         <v>10</v>
       </c>
       <c r="B242" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C242" s="2">
         <v>70</v>
@@ -3832,7 +3832,7 @@
         <v>10</v>
       </c>
       <c r="B243" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C243" s="2">
         <v>60</v>
@@ -3846,7 +3846,7 @@
         <v>10</v>
       </c>
       <c r="B244" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C244" s="2">
         <v>50</v>
@@ -3860,7 +3860,7 @@
         <v>10</v>
       </c>
       <c r="B245" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C245" s="2">
         <v>40</v>
@@ -3874,7 +3874,7 @@
         <v>10</v>
       </c>
       <c r="B246" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C246" s="2">
         <v>30</v>
@@ -3888,7 +3888,7 @@
         <v>10</v>
       </c>
       <c r="B247" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C247" s="2">
         <v>20</v>
@@ -3902,7 +3902,7 @@
         <v>10</v>
       </c>
       <c r="B248" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C248" s="2">
         <v>10</v>
@@ -3916,7 +3916,7 @@
         <v>10</v>
       </c>
       <c r="B249" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C249" s="2">
         <v>0</v>

</xml_diff>